<commit_message>
fresh mosquito tape update
</commit_message>
<xml_diff>
--- a/tapestation/mos_metadata_tidy.xlsx
+++ b/tapestation/mos_metadata_tidy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lexikeene/Documents/Research/papers/OC_Figures/Old_Collections_Figures/tapestation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31772E9-D282-1547-9EFF-11F7686E3472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29582A9B-BDF3-A046-894F-17E6E4E75272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33660" yWindow="1960" windowWidth="27240" windowHeight="15080" xr2:uid="{DE34D55F-1DB2-6046-9BF5-078AEB0E2E14}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="27240" windowHeight="15080" xr2:uid="{DE34D55F-1DB2-6046-9BF5-078AEB0E2E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="99">
   <si>
     <t>tape_id</t>
   </si>
@@ -315,6 +314,21 @@
   </si>
   <si>
     <t>m9</t>
+  </si>
+  <si>
+    <t>Fresh_F_1</t>
+  </si>
+  <si>
+    <t>Fresh_F_2</t>
+  </si>
+  <si>
+    <t>Fresh_F_3</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>m10</t>
   </si>
 </sst>
 </file>
@@ -675,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53742FEE-7E50-2340-BC3E-5A1D76934070}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2030,6 +2044,57 @@
         <v>36</v>
       </c>
     </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="1">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" s="1">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>